<commit_message>
add changes from master
</commit_message>
<xml_diff>
--- a/python/DataSets/rezh.xlsx
+++ b/python/DataSets/rezh.xlsx
@@ -61,7 +61,7 @@
     <t>623750, Свердловская область, г. Реж, улица Советская, дом №2, встроенное нежилое помещение №111</t>
   </si>
   <si>
-    <t>623750,  г. Реж Свердловской области,  улица  Максима Горького, дом №19  Помещения: №101-109.112-115</t>
+    <t>623750,  г. Реж Свердловской области,  улица  Максима Горького, дом №19</t>
   </si>
   <si>
     <t>623750, Свердловская обл., г. Реж, ул. Энгельса, д.6</t>
@@ -662,7 +662,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -672,6 +672,11 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b val="1"/>
@@ -685,7 +690,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -701,6 +706,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -846,49 +857,49 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -912,6 +923,7 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -928,10 +940,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -1108,11 +1120,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1121,7 +1136,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1136,19 +1151,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
             <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1396,12 +1411,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1692,7 +1707,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1970,19 +1985,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G146"/>
+  <dimension ref="A1:G143"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="79.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.5469" style="1" customWidth="1"/>
+    <col min="1" max="1" width="79.8516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.0156" style="1" customWidth="1"/>
-    <col min="5" max="5" width="39.8359" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40" style="1" customWidth="1"/>
+    <col min="5" max="5" width="39.8516" style="1" customWidth="1"/>
     <col min="6" max="7" width="16.3516" style="1" customWidth="1"/>
     <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
@@ -3469,7 +3482,7 @@
     </row>
     <row r="83" ht="20.7" customHeight="1">
       <c r="A83" t="s" s="5">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="B83" t="s" s="6">
         <v>65</v>
@@ -3486,7 +3499,7 @@
     </row>
     <row r="84" ht="20.7" customHeight="1">
       <c r="A84" t="s" s="5">
-        <v>64</v>
+        <v>131</v>
       </c>
       <c r="B84" t="s" s="6">
         <v>65</v>
@@ -3503,7 +3516,7 @@
     </row>
     <row r="85" ht="20.7" customHeight="1">
       <c r="A85" t="s" s="5">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B85" t="s" s="6">
         <v>65</v>
@@ -3520,7 +3533,7 @@
     </row>
     <row r="86" ht="20.7" customHeight="1">
       <c r="A86" t="s" s="5">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B86" t="s" s="6">
         <v>65</v>
@@ -3537,7 +3550,7 @@
     </row>
     <row r="87" ht="20.7" customHeight="1">
       <c r="A87" t="s" s="5">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B87" t="s" s="6">
         <v>65</v>
@@ -3554,7 +3567,7 @@
     </row>
     <row r="88" ht="20.7" customHeight="1">
       <c r="A88" t="s" s="5">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B88" t="s" s="6">
         <v>65</v>
@@ -3571,7 +3584,7 @@
     </row>
     <row r="89" ht="20.7" customHeight="1">
       <c r="A89" t="s" s="5">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B89" t="s" s="6">
         <v>65</v>
@@ -3588,7 +3601,7 @@
     </row>
     <row r="90" ht="20.7" customHeight="1">
       <c r="A90" t="s" s="5">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B90" t="s" s="6">
         <v>65</v>
@@ -3605,7 +3618,7 @@
     </row>
     <row r="91" ht="20.7" customHeight="1">
       <c r="A91" t="s" s="5">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B91" t="s" s="6">
         <v>65</v>
@@ -3622,7 +3635,7 @@
     </row>
     <row r="92" ht="20.7" customHeight="1">
       <c r="A92" t="s" s="5">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B92" t="s" s="6">
         <v>65</v>
@@ -3639,16 +3652,16 @@
     </row>
     <row r="93" ht="20.7" customHeight="1">
       <c r="A93" t="s" s="5">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B93" t="s" s="6">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="C93" t="s" s="10">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="D93" t="s" s="14">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="E93" s="15"/>
       <c r="F93" s="16"/>
@@ -3656,16 +3669,16 @@
     </row>
     <row r="94" ht="20.7" customHeight="1">
       <c r="A94" t="s" s="5">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B94" t="s" s="6">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="C94" t="s" s="10">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="D94" t="s" s="14">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="E94" s="15"/>
       <c r="F94" s="16"/>
@@ -3724,7 +3737,7 @@
     </row>
     <row r="98" ht="20.7" customHeight="1">
       <c r="A98" t="s" s="5">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B98" t="s" s="6">
         <v>14</v>
@@ -3741,7 +3754,7 @@
     </row>
     <row r="99" ht="20.7" customHeight="1">
       <c r="A99" t="s" s="5">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B99" t="s" s="6">
         <v>14</v>
@@ -3758,7 +3771,7 @@
     </row>
     <row r="100" ht="20.7" customHeight="1">
       <c r="A100" t="s" s="5">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B100" t="s" s="6">
         <v>14</v>
@@ -3792,7 +3805,7 @@
     </row>
     <row r="102" ht="20.7" customHeight="1">
       <c r="A102" t="s" s="5">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B102" t="s" s="6">
         <v>14</v>
@@ -3809,7 +3822,7 @@
     </row>
     <row r="103" ht="20.7" customHeight="1">
       <c r="A103" t="s" s="5">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B103" t="s" s="6">
         <v>14</v>
@@ -3860,10 +3873,10 @@
     </row>
     <row r="106" ht="20.7" customHeight="1">
       <c r="A106" t="s" s="5">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B106" t="s" s="6">
-        <v>14</v>
+        <v>150</v>
       </c>
       <c r="C106" t="s" s="10">
         <v>145</v>
@@ -3877,7 +3890,7 @@
     </row>
     <row r="107" ht="20.7" customHeight="1">
       <c r="A107" t="s" s="5">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B107" t="s" s="6">
         <v>14</v>
@@ -3892,35 +3905,35 @@
       <c r="F107" s="16"/>
       <c r="G107" s="12"/>
     </row>
-    <row r="108" ht="20.7" customHeight="1">
+    <row r="108" ht="32.55" customHeight="1">
       <c r="A108" t="s" s="5">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B108" t="s" s="6">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C108" t="s" s="10">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="D108" t="s" s="14">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="E108" s="15"/>
       <c r="F108" s="16"/>
       <c r="G108" s="12"/>
     </row>
-    <row r="109" ht="20.7" customHeight="1">
+    <row r="109" ht="32.55" customHeight="1">
       <c r="A109" t="s" s="5">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="B109" t="s" s="6">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="C109" t="s" s="10">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="D109" t="s" s="14">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="E109" s="15"/>
       <c r="F109" s="16"/>
@@ -3928,10 +3941,10 @@
     </row>
     <row r="110" ht="32.55" customHeight="1">
       <c r="A110" t="s" s="5">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B110" t="s" s="6">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C110" t="s" s="10">
         <v>154</v>
@@ -3948,7 +3961,7 @@
         <v>156</v>
       </c>
       <c r="B111" t="s" s="6">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C111" t="s" s="10">
         <v>154</v>
@@ -3956,16 +3969,18 @@
       <c r="D111" t="s" s="14">
         <v>155</v>
       </c>
-      <c r="E111" s="15"/>
+      <c r="E111" t="s" s="6">
+        <v>160</v>
+      </c>
       <c r="F111" s="16"/>
       <c r="G111" s="12"/>
     </row>
-    <row r="112" ht="32.55" customHeight="1">
+    <row r="112" ht="32.7" customHeight="1">
       <c r="A112" t="s" s="5">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B112" t="s" s="6">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C112" t="s" s="10">
         <v>154</v>
@@ -3973,16 +3988,18 @@
       <c r="D112" t="s" s="14">
         <v>155</v>
       </c>
-      <c r="E112" s="15"/>
+      <c r="E112" t="s" s="6">
+        <v>160</v>
+      </c>
       <c r="F112" s="16"/>
       <c r="G112" s="12"/>
     </row>
-    <row r="113" ht="32.55" customHeight="1">
+    <row r="113" ht="32.7" customHeight="1">
       <c r="A113" t="s" s="5">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B113" t="s" s="6">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C113" t="s" s="10">
         <v>154</v>
@@ -3990,18 +4007,16 @@
       <c r="D113" t="s" s="14">
         <v>155</v>
       </c>
-      <c r="E113" t="s" s="6">
-        <v>160</v>
-      </c>
+      <c r="E113" s="15"/>
       <c r="F113" s="16"/>
       <c r="G113" s="12"/>
     </row>
-    <row r="114" ht="32.7" customHeight="1">
+    <row r="114" ht="32.55" customHeight="1">
       <c r="A114" t="s" s="5">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B114" t="s" s="6">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C114" t="s" s="10">
         <v>154</v>
@@ -4009,17 +4024,17 @@
       <c r="D114" t="s" s="14">
         <v>155</v>
       </c>
-      <c r="E114" t="s" s="6">
-        <v>160</v>
-      </c>
+      <c r="E114" s="15"/>
       <c r="F114" s="16"/>
       <c r="G114" s="12"/>
     </row>
     <row r="115" ht="32.55" customHeight="1">
       <c r="A115" t="s" s="5">
-        <v>107</v>
-      </c>
-      <c r="B115" s="15"/>
+        <v>166</v>
+      </c>
+      <c r="B115" t="s" s="6">
+        <v>165</v>
+      </c>
       <c r="C115" t="s" s="10">
         <v>154</v>
       </c>
@@ -4032,10 +4047,10 @@
     </row>
     <row r="116" ht="32.7" customHeight="1">
       <c r="A116" t="s" s="5">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B116" t="s" s="6">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="C116" t="s" s="10">
         <v>154</v>
@@ -4043,16 +4058,18 @@
       <c r="D116" t="s" s="14">
         <v>155</v>
       </c>
-      <c r="E116" s="15"/>
+      <c r="E116" t="s" s="6">
+        <v>169</v>
+      </c>
       <c r="F116" s="16"/>
       <c r="G116" s="12"/>
     </row>
-    <row r="117" ht="32.55" customHeight="1">
+    <row r="117" ht="32.7" customHeight="1">
       <c r="A117" t="s" s="5">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B117" t="s" s="6">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C117" t="s" s="10">
         <v>154</v>
@@ -4060,16 +4077,18 @@
       <c r="D117" t="s" s="14">
         <v>155</v>
       </c>
-      <c r="E117" s="15"/>
+      <c r="E117" t="s" s="6">
+        <v>169</v>
+      </c>
       <c r="F117" s="16"/>
       <c r="G117" s="12"/>
     </row>
-    <row r="118" ht="32.55" customHeight="1">
+    <row r="118" ht="32.7" customHeight="1">
       <c r="A118" t="s" s="5">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B118" t="s" s="6">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C118" t="s" s="10">
         <v>154</v>
@@ -4077,13 +4096,15 @@
       <c r="D118" t="s" s="14">
         <v>155</v>
       </c>
-      <c r="E118" s="15"/>
+      <c r="E118" t="s" s="6">
+        <v>169</v>
+      </c>
       <c r="F118" s="16"/>
       <c r="G118" s="12"/>
     </row>
     <row r="119" ht="32.7" customHeight="1">
       <c r="A119" t="s" s="5">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B119" t="s" s="6">
         <v>168</v>
@@ -4102,7 +4123,7 @@
     </row>
     <row r="120" ht="32.7" customHeight="1">
       <c r="A120" t="s" s="5">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B120" t="s" s="6">
         <v>168</v>
@@ -4114,14 +4135,14 @@
         <v>155</v>
       </c>
       <c r="E120" t="s" s="6">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="F120" s="16"/>
       <c r="G120" s="12"/>
     </row>
     <row r="121" ht="32.7" customHeight="1">
       <c r="A121" t="s" s="5">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B121" t="s" s="6">
         <v>168</v>
@@ -4133,14 +4154,14 @@
         <v>155</v>
       </c>
       <c r="E121" t="s" s="6">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="F121" s="16"/>
       <c r="G121" s="12"/>
     </row>
     <row r="122" ht="32.7" customHeight="1">
       <c r="A122" t="s" s="5">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="B122" t="s" s="6">
         <v>168</v>
@@ -4152,14 +4173,14 @@
         <v>155</v>
       </c>
       <c r="E122" t="s" s="6">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="F122" s="16"/>
       <c r="G122" s="12"/>
     </row>
     <row r="123" ht="32.7" customHeight="1">
       <c r="A123" t="s" s="5">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B123" t="s" s="6">
         <v>168</v>
@@ -4171,17 +4192,17 @@
         <v>155</v>
       </c>
       <c r="E123" t="s" s="6">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="F123" s="16"/>
       <c r="G123" s="12"/>
     </row>
-    <row r="124" ht="32.7" customHeight="1">
+    <row r="124" ht="32.55" customHeight="1">
       <c r="A124" t="s" s="5">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B124" t="s" s="6">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="C124" t="s" s="10">
         <v>154</v>
@@ -4189,18 +4210,16 @@
       <c r="D124" t="s" s="14">
         <v>155</v>
       </c>
-      <c r="E124" t="s" s="6">
-        <v>176</v>
-      </c>
+      <c r="E124" s="15"/>
       <c r="F124" s="16"/>
       <c r="G124" s="12"/>
     </row>
     <row r="125" ht="32.7" customHeight="1">
       <c r="A125" t="s" s="5">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B125" t="s" s="6">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="C125" t="s" s="10">
         <v>154</v>
@@ -4209,14 +4228,14 @@
         <v>155</v>
       </c>
       <c r="E125" t="s" s="6">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="F125" s="16"/>
       <c r="G125" s="12"/>
     </row>
     <row r="126" ht="32.7" customHeight="1">
       <c r="A126" t="s" s="5">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B126" t="s" s="6">
         <v>168</v>
@@ -4228,17 +4247,17 @@
         <v>155</v>
       </c>
       <c r="E126" t="s" s="6">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="F126" s="16"/>
       <c r="G126" s="12"/>
     </row>
-    <row r="127" ht="32.55" customHeight="1">
+    <row r="127" ht="32.7" customHeight="1">
       <c r="A127" t="s" s="5">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B127" t="s" s="6">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="C127" t="s" s="10">
         <v>154</v>
@@ -4246,16 +4265,18 @@
       <c r="D127" t="s" s="14">
         <v>155</v>
       </c>
-      <c r="E127" s="15"/>
+      <c r="E127" t="s" s="6">
+        <v>169</v>
+      </c>
       <c r="F127" s="16"/>
       <c r="G127" s="12"/>
     </row>
     <row r="128" ht="32.7" customHeight="1">
       <c r="A128" t="s" s="5">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B128" t="s" s="6">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="C128" t="s" s="10">
         <v>154</v>
@@ -4264,14 +4285,14 @@
         <v>155</v>
       </c>
       <c r="E128" t="s" s="6">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="F128" s="16"/>
       <c r="G128" s="12"/>
     </row>
     <row r="129" ht="32.7" customHeight="1">
       <c r="A129" t="s" s="5">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B129" t="s" s="6">
         <v>168</v>
@@ -4290,7 +4311,7 @@
     </row>
     <row r="130" ht="32.7" customHeight="1">
       <c r="A130" t="s" s="5">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B130" t="s" s="6">
         <v>168</v>
@@ -4309,7 +4330,7 @@
     </row>
     <row r="131" ht="32.7" customHeight="1">
       <c r="A131" t="s" s="5">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B131" t="s" s="6">
         <v>168</v>
@@ -4328,7 +4349,7 @@
     </row>
     <row r="132" ht="32.7" customHeight="1">
       <c r="A132" t="s" s="5">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B132" t="s" s="6">
         <v>168</v>
@@ -4347,7 +4368,7 @@
     </row>
     <row r="133" ht="32.7" customHeight="1">
       <c r="A133" t="s" s="5">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B133" t="s" s="6">
         <v>168</v>
@@ -4364,69 +4385,63 @@
       <c r="F133" s="16"/>
       <c r="G133" s="12"/>
     </row>
-    <row r="134" ht="32.7" customHeight="1">
+    <row r="134" ht="20.7" customHeight="1">
       <c r="A134" t="s" s="5">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="B134" t="s" s="6">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="C134" t="s" s="10">
-        <v>154</v>
+        <v>193</v>
       </c>
       <c r="D134" t="s" s="14">
-        <v>155</v>
-      </c>
-      <c r="E134" t="s" s="6">
-        <v>169</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="E134" s="15"/>
       <c r="F134" s="16"/>
       <c r="G134" s="12"/>
     </row>
-    <row r="135" ht="32.7" customHeight="1">
+    <row r="135" ht="20.7" customHeight="1">
       <c r="A135" t="s" s="5">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B135" t="s" s="6">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="C135" t="s" s="10">
-        <v>154</v>
+        <v>193</v>
       </c>
       <c r="D135" t="s" s="14">
-        <v>155</v>
-      </c>
-      <c r="E135" t="s" s="6">
-        <v>169</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="E135" s="15"/>
       <c r="F135" s="16"/>
       <c r="G135" s="12"/>
     </row>
-    <row r="136" ht="32.7" customHeight="1">
+    <row r="136" ht="20.7" customHeight="1">
       <c r="A136" t="s" s="5">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B136" t="s" s="6">
-        <v>168</v>
+        <v>198</v>
       </c>
       <c r="C136" t="s" s="10">
-        <v>154</v>
+        <v>193</v>
       </c>
       <c r="D136" t="s" s="14">
-        <v>155</v>
-      </c>
-      <c r="E136" t="s" s="6">
-        <v>169</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="E136" s="15"/>
       <c r="F136" s="16"/>
       <c r="G136" s="12"/>
     </row>
     <row r="137" ht="20.7" customHeight="1">
       <c r="A137" t="s" s="5">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="B137" t="s" s="6">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C137" t="s" s="10">
         <v>193</v>
@@ -4440,10 +4455,10 @@
     </row>
     <row r="138" ht="20.7" customHeight="1">
       <c r="A138" t="s" s="5">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B138" t="s" s="6">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C138" t="s" s="10">
         <v>193</v>
@@ -4457,10 +4472,10 @@
     </row>
     <row r="139" ht="20.7" customHeight="1">
       <c r="A139" t="s" s="5">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B139" t="s" s="6">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C139" t="s" s="10">
         <v>193</v>
@@ -4474,16 +4489,16 @@
     </row>
     <row r="140" ht="20.7" customHeight="1">
       <c r="A140" t="s" s="5">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B140" t="s" s="6">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C140" t="s" s="10">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="D140" t="s" s="14">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="E140" s="15"/>
       <c r="F140" s="16"/>
@@ -4491,44 +4506,44 @@
     </row>
     <row r="141" ht="20.7" customHeight="1">
       <c r="A141" t="s" s="5">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B141" t="s" s="6">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="C141" t="s" s="10">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="D141" t="s" s="14">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="E141" s="15"/>
       <c r="F141" s="16"/>
       <c r="G141" s="12"/>
     </row>
-    <row r="142" ht="20.7" customHeight="1">
+    <row r="142" ht="32.7" customHeight="1">
       <c r="A142" t="s" s="5">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B142" t="s" s="6">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="C142" t="s" s="10">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="D142" t="s" s="14">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="E142" s="15"/>
       <c r="F142" s="16"/>
       <c r="G142" s="12"/>
     </row>
-    <row r="143" ht="20.7" customHeight="1">
+    <row r="143" ht="32.7" customHeight="1">
       <c r="A143" t="s" s="5">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="B143" t="s" s="6">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="C143" t="s" s="10">
         <v>205</v>
@@ -4539,57 +4554,6 @@
       <c r="E143" s="15"/>
       <c r="F143" s="16"/>
       <c r="G143" s="12"/>
-    </row>
-    <row r="144" ht="20.7" customHeight="1">
-      <c r="A144" t="s" s="5">
-        <v>207</v>
-      </c>
-      <c r="B144" t="s" s="6">
-        <v>208</v>
-      </c>
-      <c r="C144" t="s" s="10">
-        <v>205</v>
-      </c>
-      <c r="D144" t="s" s="14">
-        <v>206</v>
-      </c>
-      <c r="E144" s="15"/>
-      <c r="F144" s="16"/>
-      <c r="G144" s="12"/>
-    </row>
-    <row r="145" ht="32.7" customHeight="1">
-      <c r="A145" t="s" s="5">
-        <v>209</v>
-      </c>
-      <c r="B145" t="s" s="6">
-        <v>210</v>
-      </c>
-      <c r="C145" t="s" s="10">
-        <v>205</v>
-      </c>
-      <c r="D145" t="s" s="14">
-        <v>206</v>
-      </c>
-      <c r="E145" s="15"/>
-      <c r="F145" s="16"/>
-      <c r="G145" s="12"/>
-    </row>
-    <row r="146" ht="32.7" customHeight="1">
-      <c r="A146" t="s" s="5">
-        <v>211</v>
-      </c>
-      <c r="B146" t="s" s="6">
-        <v>212</v>
-      </c>
-      <c r="C146" t="s" s="10">
-        <v>205</v>
-      </c>
-      <c r="D146" t="s" s="14">
-        <v>206</v>
-      </c>
-      <c r="E146" s="15"/>
-      <c r="F146" s="16"/>
-      <c r="G146" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>